<commit_message>
Update: Se Modifica Documento
</commit_message>
<xml_diff>
--- a/6- VI_Trimestre/04- Matriz_Análisis_De_Riesgos/01-Matriz_Análisis_De_Riesgos.xlsx
+++ b/6- VI_Trimestre/04- Matriz_Análisis_De_Riesgos/01-Matriz_Análisis_De_Riesgos.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9cbba347ef89ad52/Escritorio/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andres_Olaya\Proyecto_Formativo\Kyukeisho_New\Kyukeisho_New\6- VI_Trimestre\04- Matriz_Análisis_De_Riesgos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{B397D671-B92F-40C0-B519-5F57AA217231}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1591B606-6CF4-411B-BEE8-85226E022A5E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB569A8C-620D-4C4E-A3C3-08EA7850636F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{89DC5D86-D368-4A46-9C4D-B4895C2CC949}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Matriz De Riesgo" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -72,9 +72,6 @@
     <t xml:space="preserve">VI </t>
   </si>
   <si>
-    <t>Miercoles 3 De Junio De 2020</t>
-  </si>
-  <si>
     <t>Alto</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>Tener una clara informacion de que es lo que se requiere (Esto incluye todas las partes)</t>
   </si>
   <si>
-    <t>Cuando las solicutudes no tienes sentido</t>
-  </si>
-  <si>
     <t>Molestia de los desarrolladores ya que no es algo necesario</t>
   </si>
   <si>
@@ -517,6 +511,12 @@
   </si>
   <si>
     <t>Puede darse ya que la informacion no es clara ni es claro a donde se quiere llegar</t>
+  </si>
+  <si>
+    <t>Viernes 5 De Junio De 2020</t>
+  </si>
+  <si>
+    <t>Cuando las solicitudes no tienes sentido</t>
   </si>
 </sst>
 </file>
@@ -1200,177 +1200,18 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1383,21 +1224,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1405,6 +1231,9 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1413,6 +1242,93 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1420,6 +1336,15 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1428,12 +1353,87 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1800,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA700F56-96E1-4984-AC95-8295388B3FD8}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67:C68"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,18 +1821,18 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="2:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E2" s="55" t="s">
-        <v>27</v>
-      </c>
-      <c r="F2" s="56"/>
+      <c r="E2" s="64" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="65"/>
       <c r="G2" s="9"/>
     </row>
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="68"/>
-      <c r="C3" s="69"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="58"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="80"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="67"/>
       <c r="G3" s="18"/>
     </row>
     <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1841,10 +1841,10 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="59"/>
-      <c r="F4" s="60"/>
+        <v>162</v>
+      </c>
+      <c r="E4" s="68"/>
+      <c r="F4" s="69"/>
       <c r="G4" s="18"/>
     </row>
     <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1855,8 +1855,8 @@
       <c r="D5" s="3">
         <v>1803170</v>
       </c>
-      <c r="E5" s="59"/>
-      <c r="F5" s="60"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="69"/>
       <c r="G5" s="18"/>
     </row>
     <row r="6" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1867,8 +1867,8 @@
       <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="59"/>
-      <c r="F6" s="60"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1879,8 +1879,8 @@
       <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="59"/>
-      <c r="F7" s="60"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="69"/>
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1891,8 +1891,8 @@
       <c r="D8" s="4">
         <v>43500</v>
       </c>
-      <c r="E8" s="59"/>
-      <c r="F8" s="60"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="69"/>
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1903,8 +1903,8 @@
       <c r="D9" s="4">
         <v>44000</v>
       </c>
-      <c r="E9" s="59"/>
-      <c r="F9" s="60"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="69"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1915,8 +1915,8 @@
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="61"/>
-      <c r="F10" s="62"/>
+      <c r="E10" s="70"/>
+      <c r="F10" s="71"/>
       <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1960,17 +1960,17 @@
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="66" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="67"/>
+      <c r="B16" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="77"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="5"/>
       <c r="C17" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="18"/>
@@ -1978,7 +1978,7 @@
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
       <c r="C18" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
@@ -1986,15 +1986,15 @@
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
       <c r="C19" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="73"/>
+      <c r="B20" s="42"/>
       <c r="C20" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
@@ -2006,164 +2006,164 @@
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9"/>
       <c r="B25" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="31" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C25" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="D25" s="31" t="s">
+      <c r="E25" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="31" t="s">
+      <c r="F25" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="31" t="s">
+      <c r="G25" s="73" t="s">
         <v>24</v>
       </c>
-      <c r="G25" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="H25" s="64"/>
-      <c r="I25" s="65"/>
-      <c r="J25" s="63" t="s">
-        <v>33</v>
-      </c>
-      <c r="K25" s="64"/>
-      <c r="L25" s="65"/>
+      <c r="H25" s="74"/>
+      <c r="I25" s="75"/>
+      <c r="J25" s="73" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="74"/>
+      <c r="L25" s="75"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
-      <c r="B26" s="99"/>
-      <c r="C26" s="100"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="100"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="100"/>
-      <c r="H26" s="100"/>
-      <c r="I26" s="100"/>
-      <c r="J26" s="100"/>
-      <c r="K26" s="100"/>
-      <c r="L26" s="101"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="63"/>
     </row>
     <row r="27" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="40">
         <v>1</v>
       </c>
-      <c r="C27" s="115" t="s">
+      <c r="C27" s="58" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="35" t="s">
+      <c r="E27" s="33" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="F27" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="34" t="s">
+      <c r="G27" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="49" t="s">
-        <v>32</v>
-      </c>
-      <c r="H27" s="49"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="K27" s="44"/>
-      <c r="L27" s="45"/>
+      <c r="H27" s="72"/>
+      <c r="I27" s="72"/>
+      <c r="J27" s="103" t="s">
+        <v>17</v>
+      </c>
+      <c r="K27" s="104"/>
+      <c r="L27" s="105"/>
     </row>
     <row r="28" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="40">
         <v>2</v>
       </c>
-      <c r="C28" s="116"/>
+      <c r="C28" s="59"/>
       <c r="D28" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="F28" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="F28" s="38" t="s">
+      <c r="G28" s="72" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="K28" s="44"/>
-      <c r="L28" s="45"/>
+      <c r="H28" s="72"/>
+      <c r="I28" s="72"/>
+      <c r="J28" s="103" t="s">
+        <v>17</v>
+      </c>
+      <c r="K28" s="104"/>
+      <c r="L28" s="105"/>
     </row>
     <row r="29" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="40">
         <v>3</v>
       </c>
-      <c r="C29" s="116"/>
+      <c r="C29" s="59"/>
       <c r="D29" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="E29" s="33" t="s">
+      <c r="F29" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="G29" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="G29" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="H29" s="49"/>
-      <c r="I29" s="49"/>
-      <c r="J29" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="K29" s="54"/>
-      <c r="L29" s="54"/>
+      <c r="H29" s="72"/>
+      <c r="I29" s="72"/>
+      <c r="J29" s="83" t="s">
+        <v>16</v>
+      </c>
+      <c r="K29" s="83"/>
+      <c r="L29" s="83"/>
     </row>
     <row r="30" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
       <c r="B30" s="40">
         <v>4</v>
       </c>
-      <c r="C30" s="117"/>
+      <c r="C30" s="60"/>
       <c r="D30" s="33" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="33" t="s">
+      <c r="F30" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="32" t="s">
+      <c r="G30" s="72" t="s">
         <v>43</v>
       </c>
-      <c r="G30" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="H30" s="49"/>
-      <c r="I30" s="49"/>
-      <c r="J30" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="K30" s="54"/>
-      <c r="L30" s="54"/>
+      <c r="H30" s="72"/>
+      <c r="I30" s="72"/>
+      <c r="J30" s="83" t="s">
+        <v>16</v>
+      </c>
+      <c r="K30" s="83"/>
+      <c r="L30" s="83"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
-      <c r="B31" s="112"/>
-      <c r="C31" s="113"/>
-      <c r="D31" s="113"/>
-      <c r="E31" s="113"/>
-      <c r="F31" s="113"/>
-      <c r="G31" s="113"/>
-      <c r="H31" s="113"/>
-      <c r="I31" s="113"/>
-      <c r="J31" s="113"/>
-      <c r="K31" s="113"/>
-      <c r="L31" s="114"/>
+      <c r="B31" s="54"/>
+      <c r="C31" s="55"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="55"/>
+      <c r="F31" s="55"/>
+      <c r="G31" s="55"/>
+      <c r="H31" s="55"/>
+      <c r="I31" s="55"/>
+      <c r="J31" s="55"/>
+      <c r="K31" s="55"/>
+      <c r="L31" s="56"/>
     </row>
     <row r="32" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="9"/>
@@ -2171,296 +2171,296 @@
         <v>5</v>
       </c>
       <c r="C32" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="36" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="36" t="s">
+      <c r="E32" s="36" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="36" t="s">
+      <c r="F32" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="33" t="s">
+      <c r="G32" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="G32" s="49" t="s">
-        <v>49</v>
-      </c>
-      <c r="H32" s="49"/>
-      <c r="I32" s="49"/>
-      <c r="J32" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="K32" s="50"/>
-      <c r="L32" s="50"/>
+      <c r="H32" s="72"/>
+      <c r="I32" s="72"/>
+      <c r="J32" s="82" t="s">
+        <v>17</v>
+      </c>
+      <c r="K32" s="82"/>
+      <c r="L32" s="82"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
-      <c r="B33" s="108"/>
-      <c r="C33" s="109"/>
-      <c r="D33" s="109"/>
-      <c r="E33" s="109"/>
-      <c r="F33" s="109"/>
-      <c r="G33" s="109"/>
-      <c r="H33" s="109"/>
-      <c r="I33" s="109"/>
-      <c r="J33" s="109"/>
-      <c r="K33" s="109"/>
-      <c r="L33" s="110"/>
+      <c r="B33" s="92"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="93"/>
+      <c r="G33" s="93"/>
+      <c r="H33" s="93"/>
+      <c r="I33" s="93"/>
+      <c r="J33" s="93"/>
+      <c r="K33" s="93"/>
+      <c r="L33" s="94"/>
     </row>
     <row r="34" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
       <c r="B34" s="41">
         <v>6</v>
       </c>
-      <c r="C34" s="111" t="s">
+      <c r="C34" s="53" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="E34" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="F34" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="F34" s="33" t="s">
+      <c r="G34" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="G34" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="H34" s="49"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
+      <c r="H34" s="72"/>
+      <c r="I34" s="72"/>
+      <c r="J34" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="K34" s="81"/>
+      <c r="L34" s="81"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
-      <c r="B35" s="108"/>
-      <c r="C35" s="109"/>
-      <c r="D35" s="109"/>
-      <c r="E35" s="109"/>
-      <c r="F35" s="109"/>
-      <c r="G35" s="109"/>
-      <c r="H35" s="109"/>
-      <c r="I35" s="109"/>
-      <c r="J35" s="109"/>
-      <c r="K35" s="109"/>
-      <c r="L35" s="110"/>
+      <c r="B35" s="92"/>
+      <c r="C35" s="93"/>
+      <c r="D35" s="93"/>
+      <c r="E35" s="93"/>
+      <c r="F35" s="93"/>
+      <c r="G35" s="93"/>
+      <c r="H35" s="93"/>
+      <c r="I35" s="93"/>
+      <c r="J35" s="93"/>
+      <c r="K35" s="93"/>
+      <c r="L35" s="94"/>
     </row>
     <row r="36" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
-      <c r="B36" s="102">
+      <c r="B36" s="49">
         <v>7</v>
       </c>
-      <c r="C36" s="118" t="s">
+      <c r="C36" s="90" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36" s="50" t="s">
         <v>55</v>
       </c>
-      <c r="D36" s="103" t="s">
+      <c r="E36" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="F36" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="104" t="s">
-        <v>60</v>
-      </c>
-      <c r="F36" s="105" t="s">
+      <c r="G36" s="84" t="s">
         <v>57</v>
       </c>
-      <c r="G36" s="106" t="s">
-        <v>58</v>
-      </c>
-      <c r="H36" s="106"/>
-      <c r="I36" s="106"/>
-      <c r="J36" s="107" t="s">
-        <v>19</v>
-      </c>
-      <c r="K36" s="107"/>
-      <c r="L36" s="107"/>
+      <c r="H36" s="84"/>
+      <c r="I36" s="84"/>
+      <c r="J36" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="K36" s="85"/>
+      <c r="L36" s="85"/>
     </row>
     <row r="37" spans="1:12" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="40">
         <v>8</v>
       </c>
-      <c r="C37" s="118"/>
+      <c r="C37" s="90"/>
       <c r="D37" s="35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E37" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="F37" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="G37" s="72" t="s">
         <v>61</v>
       </c>
-      <c r="F37" s="33" t="s">
-        <v>57</v>
-      </c>
-      <c r="G37" s="49" t="s">
-        <v>62</v>
-      </c>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="K37" s="47"/>
-      <c r="L37" s="48"/>
+      <c r="H37" s="72"/>
+      <c r="I37" s="72"/>
+      <c r="J37" s="106" t="s">
+        <v>16</v>
+      </c>
+      <c r="K37" s="107"/>
+      <c r="L37" s="108"/>
     </row>
     <row r="38" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="40">
         <v>9</v>
       </c>
-      <c r="C38" s="118"/>
+      <c r="C38" s="90"/>
       <c r="D38" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="E38" s="33" t="s">
+      <c r="F38" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="F38" s="36" t="s">
+      <c r="G38" s="72" t="s">
         <v>65</v>
       </c>
-      <c r="G38" s="49" t="s">
-        <v>66</v>
-      </c>
-      <c r="H38" s="49"/>
-      <c r="I38" s="49"/>
-      <c r="J38" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="K38" s="52"/>
-      <c r="L38" s="52"/>
+      <c r="H38" s="72"/>
+      <c r="I38" s="72"/>
+      <c r="J38" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="K38" s="81"/>
+      <c r="L38" s="81"/>
     </row>
     <row r="39" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="40">
         <v>10</v>
       </c>
-      <c r="C39" s="119"/>
+      <c r="C39" s="91"/>
       <c r="D39" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="E39" s="38" t="s">
+        <v>66</v>
+      </c>
+      <c r="F39" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="E39" s="38" t="s">
+      <c r="G39" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="F39" s="36" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" s="49" t="s">
-        <v>70</v>
-      </c>
-      <c r="H39" s="49"/>
-      <c r="I39" s="49"/>
-      <c r="J39" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="K39" s="51"/>
-      <c r="L39" s="51"/>
+      <c r="H39" s="72"/>
+      <c r="I39" s="72"/>
+      <c r="J39" s="88" t="s">
+        <v>16</v>
+      </c>
+      <c r="K39" s="88"/>
+      <c r="L39" s="88"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
-      <c r="B40" s="82"/>
-      <c r="C40" s="74"/>
-      <c r="D40" s="74"/>
-      <c r="E40" s="74"/>
-      <c r="F40" s="74"/>
-      <c r="G40" s="74"/>
-      <c r="H40" s="74"/>
-      <c r="I40" s="74"/>
-      <c r="J40" s="74"/>
-      <c r="K40" s="74"/>
-      <c r="L40" s="75"/>
+      <c r="B40" s="100"/>
+      <c r="C40" s="101"/>
+      <c r="D40" s="101"/>
+      <c r="E40" s="101"/>
+      <c r="F40" s="101"/>
+      <c r="G40" s="101"/>
+      <c r="H40" s="101"/>
+      <c r="I40" s="101"/>
+      <c r="J40" s="101"/>
+      <c r="K40" s="101"/>
+      <c r="L40" s="102"/>
     </row>
     <row r="41" spans="1:12" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
       <c r="B41" s="41">
         <v>11</v>
       </c>
-      <c r="C41" s="88" t="s">
+      <c r="C41" s="98" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="33" t="s">
         <v>71</v>
       </c>
-      <c r="D41" s="37" t="s">
+      <c r="F41" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="E41" s="33" t="s">
+      <c r="G41" s="72" t="s">
         <v>73</v>
       </c>
-      <c r="F41" s="36" t="s">
-        <v>74</v>
-      </c>
-      <c r="G41" s="49" t="s">
-        <v>75</v>
-      </c>
-      <c r="H41" s="49"/>
-      <c r="I41" s="49"/>
-      <c r="J41" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="K41" s="54"/>
-      <c r="L41" s="54"/>
+      <c r="H41" s="72"/>
+      <c r="I41" s="72"/>
+      <c r="J41" s="83" t="s">
+        <v>16</v>
+      </c>
+      <c r="K41" s="83"/>
+      <c r="L41" s="83"/>
     </row>
     <row r="42" spans="1:12" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="41">
         <v>12</v>
       </c>
-      <c r="C42" s="87"/>
+      <c r="C42" s="99"/>
       <c r="D42" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="E42" s="33" t="s">
+        <v>75</v>
+      </c>
+      <c r="F42" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="E42" s="33" t="s">
+      <c r="G42" s="72" t="s">
         <v>77</v>
       </c>
-      <c r="F42" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="G42" s="49" t="s">
-        <v>79</v>
-      </c>
-      <c r="H42" s="49"/>
-      <c r="I42" s="49"/>
-      <c r="J42" s="72" t="s">
-        <v>16</v>
-      </c>
-      <c r="K42" s="72"/>
-      <c r="L42" s="72"/>
+      <c r="H42" s="72"/>
+      <c r="I42" s="72"/>
+      <c r="J42" s="89" t="s">
+        <v>15</v>
+      </c>
+      <c r="K42" s="89"/>
+      <c r="L42" s="89"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="76"/>
-      <c r="C43" s="77"/>
-      <c r="D43" s="77"/>
-      <c r="E43" s="77"/>
-      <c r="F43" s="77"/>
-      <c r="G43" s="77"/>
-      <c r="H43" s="77"/>
-      <c r="I43" s="77"/>
-      <c r="J43" s="77"/>
-      <c r="K43" s="77"/>
-      <c r="L43" s="78"/>
+      <c r="B43" s="109"/>
+      <c r="C43" s="110"/>
+      <c r="D43" s="110"/>
+      <c r="E43" s="110"/>
+      <c r="F43" s="110"/>
+      <c r="G43" s="110"/>
+      <c r="H43" s="110"/>
+      <c r="I43" s="110"/>
+      <c r="J43" s="110"/>
+      <c r="K43" s="110"/>
+      <c r="L43" s="111"/>
     </row>
     <row r="44" spans="1:12" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="41">
         <v>13</v>
       </c>
       <c r="C44" s="86" t="s">
+        <v>78</v>
+      </c>
+      <c r="D44" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="33" t="s">
         <v>80</v>
       </c>
-      <c r="D44" s="36" t="s">
+      <c r="F44" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="E44" s="33" t="s">
+      <c r="G44" s="72" t="s">
         <v>82</v>
       </c>
-      <c r="F44" s="36" t="s">
-        <v>83</v>
-      </c>
-      <c r="G44" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="H44" s="49"/>
-      <c r="I44" s="49"/>
-      <c r="J44" s="54" t="s">
-        <v>17</v>
-      </c>
-      <c r="K44" s="54"/>
-      <c r="L44" s="54"/>
+      <c r="H44" s="72"/>
+      <c r="I44" s="72"/>
+      <c r="J44" s="83" t="s">
+        <v>16</v>
+      </c>
+      <c r="K44" s="83"/>
+      <c r="L44" s="83"/>
     </row>
     <row r="45" spans="1:12" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="41">
@@ -2468,24 +2468,24 @@
       </c>
       <c r="C45" s="86"/>
       <c r="D45" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E45" s="33" t="s">
+        <v>84</v>
+      </c>
+      <c r="F45" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="E45" s="33" t="s">
+      <c r="G45" s="72" t="s">
         <v>86</v>
       </c>
-      <c r="F45" s="36" t="s">
-        <v>87</v>
-      </c>
-      <c r="G45" s="49" t="s">
-        <v>88</v>
-      </c>
-      <c r="H45" s="49"/>
-      <c r="I45" s="49"/>
-      <c r="J45" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="K45" s="51"/>
-      <c r="L45" s="51"/>
+      <c r="H45" s="72"/>
+      <c r="I45" s="72"/>
+      <c r="J45" s="88" t="s">
+        <v>16</v>
+      </c>
+      <c r="K45" s="88"/>
+      <c r="L45" s="88"/>
     </row>
     <row r="46" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="41">
@@ -2493,204 +2493,204 @@
       </c>
       <c r="C46" s="86"/>
       <c r="D46" s="36" t="s">
+        <v>87</v>
+      </c>
+      <c r="E46" s="33" t="s">
+        <v>88</v>
+      </c>
+      <c r="F46" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="E46" s="33" t="s">
+      <c r="G46" s="72" t="s">
         <v>90</v>
       </c>
-      <c r="F46" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="G46" s="49" t="s">
-        <v>92</v>
-      </c>
-      <c r="H46" s="49"/>
-      <c r="I46" s="49"/>
-      <c r="J46" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="K46" s="50"/>
-      <c r="L46" s="50"/>
+      <c r="H46" s="72"/>
+      <c r="I46" s="72"/>
+      <c r="J46" s="82" t="s">
+        <v>17</v>
+      </c>
+      <c r="K46" s="82"/>
+      <c r="L46" s="82"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="79"/>
-      <c r="C47" s="80"/>
-      <c r="D47" s="80"/>
-      <c r="E47" s="80"/>
-      <c r="F47" s="80"/>
-      <c r="G47" s="80"/>
-      <c r="H47" s="80"/>
-      <c r="I47" s="80"/>
-      <c r="J47" s="80"/>
-      <c r="K47" s="80"/>
-      <c r="L47" s="81"/>
+      <c r="B47" s="43"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
+      <c r="F47" s="44"/>
+      <c r="G47" s="44"/>
+      <c r="H47" s="44"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
+      <c r="K47" s="44"/>
+      <c r="L47" s="45"/>
     </row>
     <row r="48" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B48" s="41">
         <v>16</v>
       </c>
-      <c r="C48" s="71" t="s">
+      <c r="C48" s="112" t="s">
+        <v>91</v>
+      </c>
+      <c r="D48" s="34" t="s">
+        <v>92</v>
+      </c>
+      <c r="E48" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="D48" s="34" t="s">
+      <c r="F48" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="E48" s="34" t="s">
+      <c r="G48" s="72" t="s">
         <v>95</v>
       </c>
-      <c r="F48" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="G48" s="49" t="s">
-        <v>97</v>
-      </c>
-      <c r="H48" s="49"/>
-      <c r="I48" s="49"/>
-      <c r="J48" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="K48" s="53"/>
-      <c r="L48" s="53"/>
+      <c r="H48" s="72"/>
+      <c r="I48" s="72"/>
+      <c r="J48" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="K48" s="87"/>
+      <c r="L48" s="87"/>
     </row>
     <row r="49" spans="2:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="41">
         <v>17</v>
       </c>
-      <c r="C49" s="71"/>
+      <c r="C49" s="112"/>
       <c r="D49" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="E49" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="F49" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="E49" s="33" t="s">
+      <c r="G49" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="F49" s="36" t="s">
-        <v>100</v>
-      </c>
-      <c r="G49" s="49" t="s">
-        <v>101</v>
-      </c>
-      <c r="H49" s="49"/>
-      <c r="I49" s="49"/>
-      <c r="J49" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="K49" s="50"/>
-      <c r="L49" s="50"/>
+      <c r="H49" s="72"/>
+      <c r="I49" s="72"/>
+      <c r="J49" s="82" t="s">
+        <v>17</v>
+      </c>
+      <c r="K49" s="82"/>
+      <c r="L49" s="82"/>
     </row>
     <row r="50" spans="2:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="41">
         <v>18</v>
       </c>
-      <c r="C50" s="71"/>
+      <c r="C50" s="112"/>
       <c r="D50" s="33" t="s">
+        <v>100</v>
+      </c>
+      <c r="E50" s="33" t="s">
+        <v>101</v>
+      </c>
+      <c r="F50" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="E50" s="33" t="s">
-        <v>103</v>
-      </c>
-      <c r="F50" s="36" t="s">
-        <v>104</v>
-      </c>
-      <c r="G50" s="49" t="s">
-        <v>108</v>
-      </c>
-      <c r="H50" s="49"/>
-      <c r="I50" s="49"/>
-      <c r="J50" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="K50" s="53"/>
-      <c r="L50" s="53"/>
+      <c r="G50" s="72" t="s">
+        <v>106</v>
+      </c>
+      <c r="H50" s="72"/>
+      <c r="I50" s="72"/>
+      <c r="J50" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="K50" s="87"/>
+      <c r="L50" s="87"/>
     </row>
     <row r="51" spans="2:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="41">
         <v>19</v>
       </c>
-      <c r="C51" s="71"/>
+      <c r="C51" s="112"/>
       <c r="D51" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="E51" s="33" t="s">
+        <v>104</v>
+      </c>
+      <c r="F51" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="E51" s="33" t="s">
-        <v>106</v>
-      </c>
-      <c r="F51" s="36" t="s">
+      <c r="G51" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="G51" s="49" t="s">
-        <v>109</v>
-      </c>
-      <c r="H51" s="49"/>
-      <c r="I51" s="49"/>
-      <c r="J51" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="K51" s="51"/>
-      <c r="L51" s="51"/>
+      <c r="H51" s="72"/>
+      <c r="I51" s="72"/>
+      <c r="J51" s="88" t="s">
+        <v>16</v>
+      </c>
+      <c r="K51" s="88"/>
+      <c r="L51" s="88"/>
     </row>
     <row r="52" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="41">
         <v>20</v>
       </c>
-      <c r="C52" s="71"/>
+      <c r="C52" s="112"/>
       <c r="D52" s="33" t="s">
+        <v>108</v>
+      </c>
+      <c r="E52" s="33" t="s">
+        <v>109</v>
+      </c>
+      <c r="F52" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="E52" s="33" t="s">
+      <c r="G52" s="72" t="s">
         <v>111</v>
       </c>
-      <c r="F52" s="36" t="s">
-        <v>112</v>
-      </c>
-      <c r="G52" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="H52" s="49"/>
-      <c r="I52" s="49"/>
-      <c r="J52" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="K52" s="50"/>
-      <c r="L52" s="50"/>
+      <c r="H52" s="72"/>
+      <c r="I52" s="72"/>
+      <c r="J52" s="82" t="s">
+        <v>17</v>
+      </c>
+      <c r="K52" s="82"/>
+      <c r="L52" s="82"/>
     </row>
     <row r="53" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="76"/>
-      <c r="C53" s="77"/>
-      <c r="D53" s="77"/>
-      <c r="E53" s="77"/>
-      <c r="F53" s="77"/>
-      <c r="G53" s="77"/>
-      <c r="H53" s="77"/>
-      <c r="I53" s="77"/>
-      <c r="J53" s="77"/>
-      <c r="K53" s="77"/>
-      <c r="L53" s="78"/>
+      <c r="B53" s="109"/>
+      <c r="C53" s="110"/>
+      <c r="D53" s="110"/>
+      <c r="E53" s="110"/>
+      <c r="F53" s="110"/>
+      <c r="G53" s="110"/>
+      <c r="H53" s="110"/>
+      <c r="I53" s="110"/>
+      <c r="J53" s="110"/>
+      <c r="K53" s="110"/>
+      <c r="L53" s="111"/>
     </row>
     <row r="54" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="41">
         <v>21</v>
       </c>
       <c r="C54" s="86" t="s">
+        <v>112</v>
+      </c>
+      <c r="D54" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="E54" s="33" t="s">
         <v>114</v>
       </c>
-      <c r="D54" s="33" t="s">
+      <c r="F54" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="E54" s="33" t="s">
+      <c r="G54" s="72" t="s">
         <v>116</v>
       </c>
-      <c r="F54" s="36" t="s">
-        <v>117</v>
-      </c>
-      <c r="G54" s="49" t="s">
-        <v>118</v>
-      </c>
-      <c r="H54" s="49"/>
-      <c r="I54" s="49"/>
-      <c r="J54" s="51" t="s">
-        <v>17</v>
-      </c>
-      <c r="K54" s="51"/>
-      <c r="L54" s="51"/>
+      <c r="H54" s="72"/>
+      <c r="I54" s="72"/>
+      <c r="J54" s="88" t="s">
+        <v>16</v>
+      </c>
+      <c r="K54" s="88"/>
+      <c r="L54" s="88"/>
     </row>
     <row r="55" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="41">
@@ -2698,24 +2698,24 @@
       </c>
       <c r="C55" s="86"/>
       <c r="D55" s="33" t="s">
+        <v>117</v>
+      </c>
+      <c r="E55" s="33" t="s">
         <v>119</v>
       </c>
-      <c r="E55" s="33" t="s">
+      <c r="F55" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="G55" s="72" t="s">
         <v>121</v>
       </c>
-      <c r="F55" s="36" t="s">
-        <v>122</v>
-      </c>
-      <c r="G55" s="49" t="s">
-        <v>123</v>
-      </c>
-      <c r="H55" s="49"/>
-      <c r="I55" s="49"/>
-      <c r="J55" s="52" t="s">
-        <v>16</v>
-      </c>
-      <c r="K55" s="52"/>
-      <c r="L55" s="52"/>
+      <c r="H55" s="72"/>
+      <c r="I55" s="72"/>
+      <c r="J55" s="81" t="s">
+        <v>15</v>
+      </c>
+      <c r="K55" s="81"/>
+      <c r="L55" s="81"/>
     </row>
     <row r="56" spans="2:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="41">
@@ -2723,393 +2723,374 @@
       </c>
       <c r="C56" s="86"/>
       <c r="D56" s="33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E56" s="33" t="s">
+        <v>122</v>
+      </c>
+      <c r="F56" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="F56" s="36" t="s">
-        <v>126</v>
-      </c>
-      <c r="G56" s="49" t="s">
-        <v>125</v>
-      </c>
-      <c r="H56" s="49"/>
-      <c r="I56" s="49"/>
-      <c r="J56" s="53" t="s">
-        <v>18</v>
-      </c>
-      <c r="K56" s="53"/>
-      <c r="L56" s="53"/>
+      <c r="G56" s="72" t="s">
+        <v>123</v>
+      </c>
+      <c r="H56" s="72"/>
+      <c r="I56" s="72"/>
+      <c r="J56" s="87" t="s">
+        <v>17</v>
+      </c>
+      <c r="K56" s="87"/>
+      <c r="L56" s="87"/>
     </row>
     <row r="57" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="76"/>
-      <c r="C57" s="77"/>
-      <c r="D57" s="77"/>
-      <c r="E57" s="77"/>
-      <c r="F57" s="77"/>
-      <c r="G57" s="77"/>
-      <c r="H57" s="77"/>
-      <c r="I57" s="77"/>
-      <c r="J57" s="77"/>
-      <c r="K57" s="77"/>
-      <c r="L57" s="78"/>
+      <c r="B57" s="109"/>
+      <c r="C57" s="110"/>
+      <c r="D57" s="110"/>
+      <c r="E57" s="110"/>
+      <c r="F57" s="110"/>
+      <c r="G57" s="110"/>
+      <c r="H57" s="110"/>
+      <c r="I57" s="110"/>
+      <c r="J57" s="110"/>
+      <c r="K57" s="110"/>
+      <c r="L57" s="111"/>
     </row>
     <row r="58" spans="2:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="40">
         <v>24</v>
       </c>
-      <c r="C58" s="120" t="s">
+      <c r="C58" s="95" t="s">
+        <v>125</v>
+      </c>
+      <c r="D58" s="33" t="s">
+        <v>126</v>
+      </c>
+      <c r="E58" s="33" t="s">
         <v>127</v>
       </c>
-      <c r="D58" s="33" t="s">
+      <c r="F58" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="E58" s="33" t="s">
+      <c r="G58" s="72" t="s">
         <v>129</v>
       </c>
-      <c r="F58" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="G58" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="H58" s="49"/>
-      <c r="I58" s="49"/>
-      <c r="J58" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="K58" s="50"/>
-      <c r="L58" s="50"/>
+      <c r="H58" s="72"/>
+      <c r="I58" s="72"/>
+      <c r="J58" s="82" t="s">
+        <v>17</v>
+      </c>
+      <c r="K58" s="82"/>
+      <c r="L58" s="82"/>
     </row>
     <row r="59" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="40">
         <v>25</v>
       </c>
-      <c r="C59" s="121"/>
+      <c r="C59" s="96"/>
       <c r="D59" s="33" t="s">
+        <v>130</v>
+      </c>
+      <c r="E59" s="33" t="s">
+        <v>131</v>
+      </c>
+      <c r="F59" s="36" t="s">
+        <v>134</v>
+      </c>
+      <c r="G59" s="72" t="s">
+        <v>133</v>
+      </c>
+      <c r="H59" s="72"/>
+      <c r="I59" s="72"/>
+      <c r="J59" s="88" t="s">
         <v>132</v>
       </c>
-      <c r="E59" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="F59" s="36" t="s">
-        <v>136</v>
-      </c>
-      <c r="G59" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="H59" s="49"/>
-      <c r="I59" s="49"/>
-      <c r="J59" s="51" t="s">
-        <v>134</v>
-      </c>
-      <c r="K59" s="51"/>
-      <c r="L59" s="51"/>
+      <c r="K59" s="88"/>
+      <c r="L59" s="88"/>
     </row>
     <row r="60" spans="2:12" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="40">
         <v>26</v>
       </c>
-      <c r="C60" s="122"/>
+      <c r="C60" s="97"/>
       <c r="D60" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="E60" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="F60" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="G60" s="72" t="s">
         <v>137</v>
       </c>
-      <c r="E60" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="F60" s="34" t="s">
+      <c r="H60" s="72"/>
+      <c r="I60" s="72"/>
+      <c r="J60" s="82" t="s">
+        <v>17</v>
+      </c>
+      <c r="K60" s="82"/>
+      <c r="L60" s="82"/>
+    </row>
+    <row r="61" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B61" s="61"/>
+      <c r="C61" s="62"/>
+      <c r="D61" s="62"/>
+      <c r="E61" s="62"/>
+      <c r="F61" s="62"/>
+      <c r="G61" s="62"/>
+      <c r="H61" s="62"/>
+      <c r="I61" s="62"/>
+      <c r="J61" s="62"/>
+      <c r="K61" s="62"/>
+      <c r="L61" s="63"/>
+    </row>
+    <row r="62" spans="2:12" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B62" s="46">
+        <v>27</v>
+      </c>
+      <c r="C62" s="57" t="s">
+        <v>139</v>
+      </c>
+      <c r="D62" s="36" t="s">
         <v>140</v>
       </c>
-      <c r="G60" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="H60" s="49"/>
-      <c r="I60" s="49"/>
-      <c r="J60" s="50" t="s">
-        <v>18</v>
-      </c>
-      <c r="K60" s="50"/>
-      <c r="L60" s="50"/>
-    </row>
-    <row r="61" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="99"/>
-      <c r="C61" s="100"/>
-      <c r="D61" s="100"/>
-      <c r="E61" s="100"/>
-      <c r="F61" s="100"/>
-      <c r="G61" s="100"/>
-      <c r="H61" s="100"/>
-      <c r="I61" s="100"/>
-      <c r="J61" s="100"/>
-      <c r="K61" s="100"/>
-      <c r="L61" s="101"/>
-    </row>
-    <row r="62" spans="2:12" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B62" s="83">
-        <v>27</v>
-      </c>
-      <c r="C62" s="123" t="s">
+      <c r="E62" s="36" t="s">
         <v>141</v>
       </c>
-      <c r="D62" s="36" t="s">
+      <c r="F62" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="E62" s="36" t="s">
+      <c r="G62" s="116" t="s">
         <v>143</v>
       </c>
-      <c r="F62" s="33" t="s">
+      <c r="H62" s="117"/>
+      <c r="I62" s="118"/>
+      <c r="J62" s="103" t="s">
+        <v>17</v>
+      </c>
+      <c r="K62" s="104"/>
+      <c r="L62" s="105"/>
+    </row>
+    <row r="63" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B63" s="122"/>
+      <c r="C63" s="123"/>
+      <c r="D63" s="123"/>
+      <c r="E63" s="123"/>
+      <c r="F63" s="123"/>
+      <c r="G63" s="123"/>
+      <c r="H63" s="123"/>
+      <c r="I63" s="123"/>
+      <c r="J63" s="123"/>
+      <c r="K63" s="123"/>
+      <c r="L63" s="124"/>
+    </row>
+    <row r="64" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B64" s="48">
+        <v>28</v>
+      </c>
+      <c r="C64" s="120" t="s">
         <v>144</v>
       </c>
-      <c r="G62" s="93" t="s">
+      <c r="D64" s="32" t="s">
         <v>145</v>
       </c>
-      <c r="H62" s="92"/>
-      <c r="I62" s="94"/>
-      <c r="J62" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="K62" s="44"/>
-      <c r="L62" s="45"/>
-    </row>
-    <row r="63" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="89"/>
-      <c r="C63" s="90"/>
-      <c r="D63" s="90"/>
-      <c r="E63" s="90"/>
-      <c r="F63" s="90"/>
-      <c r="G63" s="90"/>
-      <c r="H63" s="90"/>
-      <c r="I63" s="90"/>
-      <c r="J63" s="90"/>
-      <c r="K63" s="90"/>
-      <c r="L63" s="91"/>
-    </row>
-    <row r="64" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B64" s="98">
-        <v>28</v>
-      </c>
-      <c r="C64" s="124" t="s">
+      <c r="E64" s="38" t="s">
         <v>146</v>
       </c>
-      <c r="D64" s="32" t="s">
+      <c r="F64" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="E64" s="38" t="s">
+      <c r="G64" s="116" t="s">
         <v>148</v>
       </c>
-      <c r="F64" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="G64" s="93" t="s">
-        <v>150</v>
-      </c>
-      <c r="H64" s="92"/>
-      <c r="I64" s="94"/>
-      <c r="J64" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="K64" s="47"/>
-      <c r="L64" s="48"/>
+      <c r="H64" s="117"/>
+      <c r="I64" s="118"/>
+      <c r="J64" s="106" t="s">
+        <v>16</v>
+      </c>
+      <c r="K64" s="107"/>
+      <c r="L64" s="108"/>
     </row>
     <row r="65" spans="2:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="41">
         <v>29</v>
       </c>
-      <c r="C65" s="119"/>
+      <c r="C65" s="91"/>
       <c r="D65" s="35" t="s">
+        <v>149</v>
+      </c>
+      <c r="E65" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="F65" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="G65" s="116" t="s">
         <v>151</v>
       </c>
-      <c r="E65" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="F65" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="G65" s="93" t="s">
-        <v>153</v>
-      </c>
-      <c r="H65" s="92"/>
-      <c r="I65" s="94"/>
-      <c r="J65" s="95" t="s">
-        <v>16</v>
-      </c>
-      <c r="K65" s="96"/>
-      <c r="L65" s="97"/>
+      <c r="H65" s="117"/>
+      <c r="I65" s="118"/>
+      <c r="J65" s="113" t="s">
+        <v>15</v>
+      </c>
+      <c r="K65" s="114"/>
+      <c r="L65" s="115"/>
     </row>
     <row r="66" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="99"/>
-      <c r="C66" s="100"/>
-      <c r="D66" s="100"/>
-      <c r="E66" s="100"/>
-      <c r="F66" s="100"/>
-      <c r="G66" s="100"/>
-      <c r="H66" s="100"/>
-      <c r="I66" s="100"/>
-      <c r="J66" s="100"/>
-      <c r="K66" s="100"/>
-      <c r="L66" s="101"/>
+      <c r="B66" s="61"/>
+      <c r="C66" s="62"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="62"/>
+      <c r="F66" s="62"/>
+      <c r="G66" s="62"/>
+      <c r="H66" s="62"/>
+      <c r="I66" s="62"/>
+      <c r="J66" s="62"/>
+      <c r="K66" s="62"/>
+      <c r="L66" s="63"/>
     </row>
     <row r="67" spans="2:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="40">
         <v>30</v>
       </c>
-      <c r="C67" s="124" t="s">
+      <c r="C67" s="120" t="s">
+        <v>153</v>
+      </c>
+      <c r="D67" s="35" t="s">
+        <v>154</v>
+      </c>
+      <c r="E67" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="D67" s="35" t="s">
+      <c r="F67" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="G67" s="116" t="s">
         <v>156</v>
       </c>
-      <c r="E67" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="F67" s="34" t="s">
-        <v>159</v>
-      </c>
-      <c r="G67" s="93" t="s">
-        <v>158</v>
-      </c>
-      <c r="H67" s="92"/>
-      <c r="I67" s="94"/>
-      <c r="J67" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="K67" s="47"/>
-      <c r="L67" s="48"/>
+      <c r="H67" s="117"/>
+      <c r="I67" s="118"/>
+      <c r="J67" s="106" t="s">
+        <v>16</v>
+      </c>
+      <c r="K67" s="107"/>
+      <c r="L67" s="108"/>
     </row>
     <row r="68" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="40">
         <v>31</v>
       </c>
-      <c r="C68" s="119"/>
+      <c r="C68" s="91"/>
       <c r="D68" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="E68" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="F68" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="G68" s="119" t="s">
         <v>160</v>
       </c>
-      <c r="E68" s="84" t="s">
-        <v>161</v>
-      </c>
-      <c r="F68" s="34" t="s">
-        <v>163</v>
-      </c>
-      <c r="G68" s="85" t="s">
-        <v>162</v>
-      </c>
-      <c r="H68" s="85"/>
-      <c r="I68" s="85"/>
-      <c r="J68" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="K68" s="44"/>
-      <c r="L68" s="45"/>
+      <c r="H68" s="119"/>
+      <c r="I68" s="119"/>
+      <c r="J68" s="103" t="s">
+        <v>17</v>
+      </c>
+      <c r="K68" s="104"/>
+      <c r="L68" s="105"/>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G69" s="42"/>
-      <c r="H69" s="42"/>
-      <c r="I69" s="42"/>
-      <c r="J69" s="42"/>
-      <c r="K69" s="42"/>
-      <c r="L69" s="42"/>
+      <c r="G69" s="121"/>
+      <c r="H69" s="121"/>
+      <c r="I69" s="121"/>
+      <c r="J69" s="121"/>
+      <c r="K69" s="121"/>
+      <c r="L69" s="121"/>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G70" s="42"/>
-      <c r="H70" s="42"/>
-      <c r="I70" s="42"/>
-      <c r="J70" s="42"/>
-      <c r="K70" s="42"/>
-      <c r="L70" s="42"/>
+      <c r="G70" s="121"/>
+      <c r="H70" s="121"/>
+      <c r="I70" s="121"/>
+      <c r="J70" s="121"/>
+      <c r="K70" s="121"/>
+      <c r="L70" s="121"/>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G71" s="42"/>
-      <c r="H71" s="42"/>
-      <c r="I71" s="42"/>
-      <c r="J71" s="42"/>
-      <c r="K71" s="42"/>
-      <c r="L71" s="42"/>
+      <c r="G71" s="121"/>
+      <c r="H71" s="121"/>
+      <c r="I71" s="121"/>
+      <c r="J71" s="121"/>
+      <c r="K71" s="121"/>
+      <c r="L71" s="121"/>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G72" s="42"/>
-      <c r="H72" s="42"/>
-      <c r="I72" s="42"/>
-      <c r="J72" s="42"/>
-      <c r="K72" s="42"/>
-      <c r="L72" s="42"/>
+      <c r="G72" s="121"/>
+      <c r="H72" s="121"/>
+      <c r="I72" s="121"/>
+      <c r="J72" s="121"/>
+      <c r="K72" s="121"/>
+      <c r="L72" s="121"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G73" s="42"/>
-      <c r="H73" s="42"/>
-      <c r="I73" s="42"/>
-      <c r="J73" s="42"/>
-      <c r="K73" s="42"/>
-      <c r="L73" s="42"/>
+      <c r="G73" s="121"/>
+      <c r="H73" s="121"/>
+      <c r="I73" s="121"/>
+      <c r="J73" s="121"/>
+      <c r="K73" s="121"/>
+      <c r="L73" s="121"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G74" s="42"/>
-      <c r="H74" s="42"/>
-      <c r="I74" s="42"/>
-      <c r="J74" s="42"/>
-      <c r="K74" s="42"/>
-      <c r="L74" s="42"/>
+      <c r="G74" s="121"/>
+      <c r="H74" s="121"/>
+      <c r="I74" s="121"/>
+      <c r="J74" s="121"/>
+      <c r="K74" s="121"/>
+      <c r="L74" s="121"/>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J75" s="42"/>
-      <c r="K75" s="42"/>
-      <c r="L75" s="42"/>
+      <c r="J75" s="121"/>
+      <c r="K75" s="121"/>
+      <c r="L75" s="121"/>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J76" s="42"/>
-      <c r="K76" s="42"/>
-      <c r="L76" s="42"/>
+      <c r="J76" s="121"/>
+      <c r="K76" s="121"/>
+      <c r="L76" s="121"/>
     </row>
   </sheetData>
   <mergeCells count="101">
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F10"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="J36:L36"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="J48:L48"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="B33:L33"/>
-    <mergeCell ref="J54:L54"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="J49:L49"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="J51:L51"/>
-    <mergeCell ref="J50:L50"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="J76:L76"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="B63:L63"/>
+    <mergeCell ref="J71:L71"/>
+    <mergeCell ref="J72:L72"/>
+    <mergeCell ref="J73:L73"/>
+    <mergeCell ref="J74:L74"/>
+    <mergeCell ref="J75:L75"/>
+    <mergeCell ref="J67:L67"/>
+    <mergeCell ref="J68:L68"/>
+    <mergeCell ref="J69:L69"/>
+    <mergeCell ref="J70:L70"/>
+    <mergeCell ref="G69:I69"/>
+    <mergeCell ref="G70:I70"/>
+    <mergeCell ref="G71:I71"/>
+    <mergeCell ref="G72:I72"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="J62:L62"/>
+    <mergeCell ref="J64:L64"/>
+    <mergeCell ref="J65:L65"/>
+    <mergeCell ref="B61:L61"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="B66:L66"/>
     <mergeCell ref="C58:C60"/>
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="B40:L40"/>
@@ -3134,35 +3115,54 @@
     <mergeCell ref="G52:I52"/>
     <mergeCell ref="C48:C52"/>
     <mergeCell ref="G54:I54"/>
-    <mergeCell ref="J62:L62"/>
-    <mergeCell ref="J64:L64"/>
-    <mergeCell ref="J65:L65"/>
-    <mergeCell ref="B61:L61"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="B66:L66"/>
-    <mergeCell ref="J76:L76"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="B63:L63"/>
-    <mergeCell ref="J71:L71"/>
-    <mergeCell ref="J72:L72"/>
-    <mergeCell ref="J73:L73"/>
-    <mergeCell ref="J74:L74"/>
-    <mergeCell ref="J75:L75"/>
-    <mergeCell ref="J67:L67"/>
-    <mergeCell ref="J68:L68"/>
-    <mergeCell ref="J69:L69"/>
-    <mergeCell ref="J70:L70"/>
-    <mergeCell ref="G69:I69"/>
-    <mergeCell ref="G70:I70"/>
-    <mergeCell ref="G71:I71"/>
-    <mergeCell ref="G72:I72"/>
-    <mergeCell ref="G73:I73"/>
-    <mergeCell ref="G74:I74"/>
+    <mergeCell ref="J54:L54"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="J49:L49"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="J51:L51"/>
+    <mergeCell ref="J50:L50"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="J46:L46"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="J48:L48"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F10"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="B33:L33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Update: Se Modifica Matriz De Riesgo Y De Calidad
</commit_message>
<xml_diff>
--- a/6- VI_Trimestre/04- Matriz_Análisis_De_Riesgos/01-Matriz_Análisis_De_Riesgos.xlsx
+++ b/6- VI_Trimestre/04- Matriz_Análisis_De_Riesgos/01-Matriz_Análisis_De_Riesgos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Andres_Olaya\Proyecto_Formativo\Kyukeisho_New\Kyukeisho_New\6- VI_Trimestre\04- Matriz_Análisis_De_Riesgos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB569A8C-620D-4C4E-A3C3-08EA7850636F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FC4867A-5122-40EA-9650-2412797C6EB1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{89DC5D86-D368-4A46-9C4D-B4895C2CC949}"/>
   </bookViews>
@@ -513,10 +513,10 @@
     <t>Puede darse ya que la informacion no es clara ni es claro a donde se quiere llegar</t>
   </si>
   <si>
-    <t>Viernes 5 De Junio De 2020</t>
-  </si>
-  <si>
     <t>Cuando las solicitudes no tienes sentido</t>
+  </si>
+  <si>
+    <t>Miércoles 3 Viernes 5 De Junio De 2020</t>
   </si>
 </sst>
 </file>
@@ -1234,13 +1234,49 @@
     <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1252,6 +1288,99 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1276,9 +1405,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1303,136 +1429,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1800,8 +1800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA700F56-96E1-4984-AC95-8295388B3FD8}">
   <dimension ref="A1:L76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1821,18 +1821,18 @@
       <c r="G1" s="9"/>
     </row>
     <row r="2" spans="2:7" ht="23.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E2" s="64" t="s">
+      <c r="E2" s="107" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="65"/>
+      <c r="F2" s="108"/>
       <c r="G2" s="9"/>
     </row>
     <row r="3" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="80"/>
-      <c r="E3" s="66"/>
-      <c r="F3" s="67"/>
+      <c r="B3" s="120"/>
+      <c r="C3" s="121"/>
+      <c r="D3" s="122"/>
+      <c r="E3" s="109"/>
+      <c r="F3" s="110"/>
       <c r="G3" s="18"/>
     </row>
     <row r="4" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1841,10 +1841,10 @@
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="E4" s="68"/>
-      <c r="F4" s="69"/>
+        <v>163</v>
+      </c>
+      <c r="E4" s="111"/>
+      <c r="F4" s="112"/>
       <c r="G4" s="18"/>
     </row>
     <row r="5" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1855,8 +1855,8 @@
       <c r="D5" s="3">
         <v>1803170</v>
       </c>
-      <c r="E5" s="68"/>
-      <c r="F5" s="69"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="112"/>
       <c r="G5" s="18"/>
     </row>
     <row r="6" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1867,8 +1867,8 @@
       <c r="D6" s="3">
         <v>1</v>
       </c>
-      <c r="E6" s="68"/>
-      <c r="F6" s="69"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="112"/>
       <c r="G6" s="18"/>
     </row>
     <row r="7" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1879,8 +1879,8 @@
       <c r="D7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="68"/>
-      <c r="F7" s="69"/>
+      <c r="E7" s="111"/>
+      <c r="F7" s="112"/>
       <c r="G7" s="18"/>
     </row>
     <row r="8" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1891,8 +1891,8 @@
       <c r="D8" s="4">
         <v>43500</v>
       </c>
-      <c r="E8" s="68"/>
-      <c r="F8" s="69"/>
+      <c r="E8" s="111"/>
+      <c r="F8" s="112"/>
       <c r="G8" s="18"/>
     </row>
     <row r="9" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1903,8 +1903,8 @@
       <c r="D9" s="4">
         <v>44000</v>
       </c>
-      <c r="E9" s="68"/>
-      <c r="F9" s="69"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="112"/>
       <c r="G9" s="18"/>
     </row>
     <row r="10" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1915,8 +1915,8 @@
       <c r="D10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E10" s="70"/>
-      <c r="F10" s="71"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="114"/>
       <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
@@ -1960,10 +1960,10 @@
       <c r="E15" s="18"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="76" t="s">
+      <c r="B16" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="77"/>
+      <c r="C16" s="119"/>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
     </row>
@@ -2020,37 +2020,37 @@
       <c r="F25" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="G25" s="73" t="s">
+      <c r="G25" s="115" t="s">
         <v>24</v>
       </c>
-      <c r="H25" s="74"/>
-      <c r="I25" s="75"/>
-      <c r="J25" s="73" t="s">
+      <c r="H25" s="116"/>
+      <c r="I25" s="117"/>
+      <c r="J25" s="115" t="s">
         <v>32</v>
       </c>
-      <c r="K25" s="74"/>
-      <c r="L25" s="75"/>
+      <c r="K25" s="116"/>
+      <c r="L25" s="117"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
-      <c r="B26" s="61"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="63"/>
+      <c r="B26" s="73"/>
+      <c r="C26" s="74"/>
+      <c r="D26" s="74"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="74"/>
+      <c r="H26" s="74"/>
+      <c r="I26" s="74"/>
+      <c r="J26" s="74"/>
+      <c r="K26" s="74"/>
+      <c r="L26" s="75"/>
     </row>
     <row r="27" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9"/>
       <c r="B27" s="40">
         <v>1</v>
       </c>
-      <c r="C27" s="58" t="s">
+      <c r="C27" s="104" t="s">
         <v>27</v>
       </c>
       <c r="D27" s="35" t="s">
@@ -2062,23 +2062,23 @@
       <c r="F27" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="G27" s="72" t="s">
+      <c r="G27" s="91" t="s">
         <v>31</v>
       </c>
-      <c r="H27" s="72"/>
-      <c r="I27" s="72"/>
-      <c r="J27" s="103" t="s">
+      <c r="H27" s="91"/>
+      <c r="I27" s="91"/>
+      <c r="J27" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="104"/>
-      <c r="L27" s="105"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="69"/>
     </row>
     <row r="28" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9"/>
       <c r="B28" s="40">
         <v>2</v>
       </c>
-      <c r="C28" s="59"/>
+      <c r="C28" s="105"/>
       <c r="D28" s="35" t="s">
         <v>33</v>
       </c>
@@ -2088,23 +2088,23 @@
       <c r="F28" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="G28" s="72" t="s">
+      <c r="G28" s="91" t="s">
         <v>35</v>
       </c>
-      <c r="H28" s="72"/>
-      <c r="I28" s="72"/>
-      <c r="J28" s="103" t="s">
+      <c r="H28" s="91"/>
+      <c r="I28" s="91"/>
+      <c r="J28" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="104"/>
-      <c r="L28" s="105"/>
+      <c r="K28" s="68"/>
+      <c r="L28" s="69"/>
     </row>
     <row r="29" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9"/>
       <c r="B29" s="40">
         <v>3</v>
       </c>
-      <c r="C29" s="59"/>
+      <c r="C29" s="105"/>
       <c r="D29" s="35" t="s">
         <v>36</v>
       </c>
@@ -2114,23 +2114,23 @@
       <c r="F29" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="G29" s="72" t="s">
+      <c r="G29" s="91" t="s">
         <v>39</v>
       </c>
-      <c r="H29" s="72"/>
-      <c r="I29" s="72"/>
-      <c r="J29" s="83" t="s">
+      <c r="H29" s="91"/>
+      <c r="I29" s="91"/>
+      <c r="J29" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="K29" s="83"/>
-      <c r="L29" s="83"/>
+      <c r="K29" s="98"/>
+      <c r="L29" s="98"/>
     </row>
     <row r="30" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="9"/>
       <c r="B30" s="40">
         <v>4</v>
       </c>
-      <c r="C30" s="60"/>
+      <c r="C30" s="106"/>
       <c r="D30" s="33" t="s">
         <v>40</v>
       </c>
@@ -2140,16 +2140,16 @@
       <c r="F30" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="72" t="s">
+      <c r="G30" s="91" t="s">
         <v>43</v>
       </c>
-      <c r="H30" s="72"/>
-      <c r="I30" s="72"/>
-      <c r="J30" s="83" t="s">
+      <c r="H30" s="91"/>
+      <c r="I30" s="91"/>
+      <c r="J30" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="K30" s="83"/>
-      <c r="L30" s="83"/>
+      <c r="K30" s="98"/>
+      <c r="L30" s="98"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="9"/>
@@ -2182,30 +2182,30 @@
       <c r="F32" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="G32" s="72" t="s">
+      <c r="G32" s="91" t="s">
         <v>48</v>
       </c>
-      <c r="H32" s="72"/>
-      <c r="I32" s="72"/>
-      <c r="J32" s="82" t="s">
+      <c r="H32" s="91"/>
+      <c r="I32" s="91"/>
+      <c r="J32" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="K32" s="82"/>
-      <c r="L32" s="82"/>
+      <c r="K32" s="92"/>
+      <c r="L32" s="92"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="9"/>
-      <c r="B33" s="92"/>
-      <c r="C33" s="93"/>
-      <c r="D33" s="93"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="93"/>
-      <c r="G33" s="93"/>
-      <c r="H33" s="93"/>
-      <c r="I33" s="93"/>
-      <c r="J33" s="93"/>
-      <c r="K33" s="93"/>
-      <c r="L33" s="94"/>
+      <c r="B33" s="101"/>
+      <c r="C33" s="102"/>
+      <c r="D33" s="102"/>
+      <c r="E33" s="102"/>
+      <c r="F33" s="102"/>
+      <c r="G33" s="102"/>
+      <c r="H33" s="102"/>
+      <c r="I33" s="102"/>
+      <c r="J33" s="102"/>
+      <c r="K33" s="102"/>
+      <c r="L33" s="103"/>
     </row>
     <row r="34" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="9"/>
@@ -2224,37 +2224,37 @@
       <c r="F34" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="G34" s="72" t="s">
+      <c r="G34" s="91" t="s">
         <v>53</v>
       </c>
-      <c r="H34" s="72"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="81" t="s">
+      <c r="H34" s="91"/>
+      <c r="I34" s="91"/>
+      <c r="J34" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="K34" s="81"/>
-      <c r="L34" s="81"/>
+      <c r="K34" s="94"/>
+      <c r="L34" s="94"/>
     </row>
     <row r="35" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="9"/>
-      <c r="B35" s="92"/>
-      <c r="C35" s="93"/>
-      <c r="D35" s="93"/>
-      <c r="E35" s="93"/>
-      <c r="F35" s="93"/>
-      <c r="G35" s="93"/>
-      <c r="H35" s="93"/>
-      <c r="I35" s="93"/>
-      <c r="J35" s="93"/>
-      <c r="K35" s="93"/>
-      <c r="L35" s="94"/>
+      <c r="B35" s="101"/>
+      <c r="C35" s="102"/>
+      <c r="D35" s="102"/>
+      <c r="E35" s="102"/>
+      <c r="F35" s="102"/>
+      <c r="G35" s="102"/>
+      <c r="H35" s="102"/>
+      <c r="I35" s="102"/>
+      <c r="J35" s="102"/>
+      <c r="K35" s="102"/>
+      <c r="L35" s="103"/>
     </row>
     <row r="36" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="49">
         <v>7</v>
       </c>
-      <c r="C36" s="90" t="s">
+      <c r="C36" s="100" t="s">
         <v>54</v>
       </c>
       <c r="D36" s="50" t="s">
@@ -2266,23 +2266,23 @@
       <c r="F36" s="52" t="s">
         <v>56</v>
       </c>
-      <c r="G36" s="84" t="s">
+      <c r="G36" s="123" t="s">
         <v>57</v>
       </c>
-      <c r="H36" s="84"/>
-      <c r="I36" s="84"/>
-      <c r="J36" s="85" t="s">
+      <c r="H36" s="123"/>
+      <c r="I36" s="123"/>
+      <c r="J36" s="124" t="s">
         <v>18</v>
       </c>
-      <c r="K36" s="85"/>
-      <c r="L36" s="85"/>
+      <c r="K36" s="124"/>
+      <c r="L36" s="124"/>
     </row>
     <row r="37" spans="1:12" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9"/>
       <c r="B37" s="40">
         <v>8</v>
       </c>
-      <c r="C37" s="90"/>
+      <c r="C37" s="100"/>
       <c r="D37" s="35" t="s">
         <v>58</v>
       </c>
@@ -2292,23 +2292,23 @@
       <c r="F37" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="G37" s="72" t="s">
+      <c r="G37" s="91" t="s">
         <v>61</v>
       </c>
-      <c r="H37" s="72"/>
-      <c r="I37" s="72"/>
-      <c r="J37" s="106" t="s">
+      <c r="H37" s="91"/>
+      <c r="I37" s="91"/>
+      <c r="J37" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="K37" s="107"/>
-      <c r="L37" s="108"/>
+      <c r="K37" s="65"/>
+      <c r="L37" s="66"/>
     </row>
     <row r="38" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9"/>
       <c r="B38" s="40">
         <v>9</v>
       </c>
-      <c r="C38" s="90"/>
+      <c r="C38" s="100"/>
       <c r="D38" s="35" t="s">
         <v>62</v>
       </c>
@@ -2318,25 +2318,25 @@
       <c r="F38" s="36" t="s">
         <v>64</v>
       </c>
-      <c r="G38" s="72" t="s">
+      <c r="G38" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="H38" s="72"/>
-      <c r="I38" s="72"/>
-      <c r="J38" s="81" t="s">
+      <c r="H38" s="91"/>
+      <c r="I38" s="91"/>
+      <c r="J38" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="K38" s="81"/>
-      <c r="L38" s="81"/>
+      <c r="K38" s="94"/>
+      <c r="L38" s="94"/>
     </row>
     <row r="39" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="9"/>
       <c r="B39" s="40">
         <v>10</v>
       </c>
-      <c r="C39" s="91"/>
+      <c r="C39" s="60"/>
       <c r="D39" s="37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E39" s="38" t="s">
         <v>66</v>
@@ -2344,37 +2344,37 @@
       <c r="F39" s="36" t="s">
         <v>67</v>
       </c>
-      <c r="G39" s="72" t="s">
+      <c r="G39" s="91" t="s">
         <v>68</v>
       </c>
-      <c r="H39" s="72"/>
-      <c r="I39" s="72"/>
-      <c r="J39" s="88" t="s">
+      <c r="H39" s="91"/>
+      <c r="I39" s="91"/>
+      <c r="J39" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="K39" s="88"/>
-      <c r="L39" s="88"/>
+      <c r="K39" s="93"/>
+      <c r="L39" s="93"/>
     </row>
     <row r="40" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="9"/>
-      <c r="B40" s="100"/>
-      <c r="C40" s="101"/>
-      <c r="D40" s="101"/>
-      <c r="E40" s="101"/>
-      <c r="F40" s="101"/>
-      <c r="G40" s="101"/>
-      <c r="H40" s="101"/>
-      <c r="I40" s="101"/>
-      <c r="J40" s="101"/>
-      <c r="K40" s="101"/>
-      <c r="L40" s="102"/>
+      <c r="B40" s="85"/>
+      <c r="C40" s="86"/>
+      <c r="D40" s="86"/>
+      <c r="E40" s="86"/>
+      <c r="F40" s="86"/>
+      <c r="G40" s="86"/>
+      <c r="H40" s="86"/>
+      <c r="I40" s="86"/>
+      <c r="J40" s="86"/>
+      <c r="K40" s="86"/>
+      <c r="L40" s="87"/>
     </row>
     <row r="41" spans="1:12" ht="45.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="9"/>
       <c r="B41" s="41">
         <v>11</v>
       </c>
-      <c r="C41" s="98" t="s">
+      <c r="C41" s="83" t="s">
         <v>69</v>
       </c>
       <c r="D41" s="37" t="s">
@@ -2386,22 +2386,22 @@
       <c r="F41" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="G41" s="72" t="s">
+      <c r="G41" s="91" t="s">
         <v>73</v>
       </c>
-      <c r="H41" s="72"/>
-      <c r="I41" s="72"/>
-      <c r="J41" s="83" t="s">
+      <c r="H41" s="91"/>
+      <c r="I41" s="91"/>
+      <c r="J41" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="K41" s="83"/>
-      <c r="L41" s="83"/>
+      <c r="K41" s="98"/>
+      <c r="L41" s="98"/>
     </row>
     <row r="42" spans="1:12" ht="83.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="41">
         <v>12</v>
       </c>
-      <c r="C42" s="99"/>
+      <c r="C42" s="84"/>
       <c r="D42" s="37" t="s">
         <v>74</v>
       </c>
@@ -2411,35 +2411,35 @@
       <c r="F42" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="72" t="s">
+      <c r="G42" s="91" t="s">
         <v>77</v>
       </c>
-      <c r="H42" s="72"/>
-      <c r="I42" s="72"/>
-      <c r="J42" s="89" t="s">
+      <c r="H42" s="91"/>
+      <c r="I42" s="91"/>
+      <c r="J42" s="99" t="s">
         <v>15</v>
       </c>
-      <c r="K42" s="89"/>
-      <c r="L42" s="89"/>
+      <c r="K42" s="99"/>
+      <c r="L42" s="99"/>
     </row>
     <row r="43" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="109"/>
-      <c r="C43" s="110"/>
-      <c r="D43" s="110"/>
-      <c r="E43" s="110"/>
-      <c r="F43" s="110"/>
-      <c r="G43" s="110"/>
-      <c r="H43" s="110"/>
-      <c r="I43" s="110"/>
-      <c r="J43" s="110"/>
-      <c r="K43" s="110"/>
-      <c r="L43" s="111"/>
+      <c r="B43" s="88"/>
+      <c r="C43" s="89"/>
+      <c r="D43" s="89"/>
+      <c r="E43" s="89"/>
+      <c r="F43" s="89"/>
+      <c r="G43" s="89"/>
+      <c r="H43" s="89"/>
+      <c r="I43" s="89"/>
+      <c r="J43" s="89"/>
+      <c r="K43" s="89"/>
+      <c r="L43" s="90"/>
     </row>
     <row r="44" spans="1:12" ht="78.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B44" s="41">
         <v>13</v>
       </c>
-      <c r="C44" s="86" t="s">
+      <c r="C44" s="95" t="s">
         <v>78</v>
       </c>
       <c r="D44" s="36" t="s">
@@ -2451,22 +2451,22 @@
       <c r="F44" s="36" t="s">
         <v>81</v>
       </c>
-      <c r="G44" s="72" t="s">
+      <c r="G44" s="91" t="s">
         <v>82</v>
       </c>
-      <c r="H44" s="72"/>
-      <c r="I44" s="72"/>
-      <c r="J44" s="83" t="s">
+      <c r="H44" s="91"/>
+      <c r="I44" s="91"/>
+      <c r="J44" s="98" t="s">
         <v>16</v>
       </c>
-      <c r="K44" s="83"/>
-      <c r="L44" s="83"/>
+      <c r="K44" s="98"/>
+      <c r="L44" s="98"/>
     </row>
     <row r="45" spans="1:12" ht="91.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B45" s="41">
         <v>14</v>
       </c>
-      <c r="C45" s="86"/>
+      <c r="C45" s="95"/>
       <c r="D45" s="35" t="s">
         <v>83</v>
       </c>
@@ -2476,22 +2476,22 @@
       <c r="F45" s="36" t="s">
         <v>85</v>
       </c>
-      <c r="G45" s="72" t="s">
+      <c r="G45" s="91" t="s">
         <v>86</v>
       </c>
-      <c r="H45" s="72"/>
-      <c r="I45" s="72"/>
-      <c r="J45" s="88" t="s">
+      <c r="H45" s="91"/>
+      <c r="I45" s="91"/>
+      <c r="J45" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="K45" s="88"/>
-      <c r="L45" s="88"/>
+      <c r="K45" s="93"/>
+      <c r="L45" s="93"/>
     </row>
     <row r="46" spans="1:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B46" s="41">
         <v>15</v>
       </c>
-      <c r="C46" s="86"/>
+      <c r="C46" s="95"/>
       <c r="D46" s="36" t="s">
         <v>87</v>
       </c>
@@ -2501,16 +2501,16 @@
       <c r="F46" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="G46" s="72" t="s">
+      <c r="G46" s="91" t="s">
         <v>90</v>
       </c>
-      <c r="H46" s="72"/>
-      <c r="I46" s="72"/>
-      <c r="J46" s="82" t="s">
+      <c r="H46" s="91"/>
+      <c r="I46" s="91"/>
+      <c r="J46" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="K46" s="82"/>
-      <c r="L46" s="82"/>
+      <c r="K46" s="92"/>
+      <c r="L46" s="92"/>
     </row>
     <row r="47" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B47" s="43"/>
@@ -2529,7 +2529,7 @@
       <c r="B48" s="41">
         <v>16</v>
       </c>
-      <c r="C48" s="112" t="s">
+      <c r="C48" s="97" t="s">
         <v>91</v>
       </c>
       <c r="D48" s="34" t="s">
@@ -2541,22 +2541,22 @@
       <c r="F48" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="G48" s="72" t="s">
+      <c r="G48" s="91" t="s">
         <v>95</v>
       </c>
-      <c r="H48" s="72"/>
-      <c r="I48" s="72"/>
-      <c r="J48" s="87" t="s">
+      <c r="H48" s="91"/>
+      <c r="I48" s="91"/>
+      <c r="J48" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="K48" s="87"/>
-      <c r="L48" s="87"/>
+      <c r="K48" s="96"/>
+      <c r="L48" s="96"/>
     </row>
     <row r="49" spans="2:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B49" s="41">
         <v>17</v>
       </c>
-      <c r="C49" s="112"/>
+      <c r="C49" s="97"/>
       <c r="D49" s="35" t="s">
         <v>96</v>
       </c>
@@ -2566,22 +2566,22 @@
       <c r="F49" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="G49" s="72" t="s">
+      <c r="G49" s="91" t="s">
         <v>99</v>
       </c>
-      <c r="H49" s="72"/>
-      <c r="I49" s="72"/>
-      <c r="J49" s="82" t="s">
+      <c r="H49" s="91"/>
+      <c r="I49" s="91"/>
+      <c r="J49" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="K49" s="82"/>
-      <c r="L49" s="82"/>
+      <c r="K49" s="92"/>
+      <c r="L49" s="92"/>
     </row>
     <row r="50" spans="2:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B50" s="41">
         <v>18</v>
       </c>
-      <c r="C50" s="112"/>
+      <c r="C50" s="97"/>
       <c r="D50" s="33" t="s">
         <v>100</v>
       </c>
@@ -2591,22 +2591,22 @@
       <c r="F50" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="G50" s="72" t="s">
+      <c r="G50" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="H50" s="72"/>
-      <c r="I50" s="72"/>
-      <c r="J50" s="87" t="s">
+      <c r="H50" s="91"/>
+      <c r="I50" s="91"/>
+      <c r="J50" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="K50" s="87"/>
-      <c r="L50" s="87"/>
+      <c r="K50" s="96"/>
+      <c r="L50" s="96"/>
     </row>
     <row r="51" spans="2:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B51" s="41">
         <v>19</v>
       </c>
-      <c r="C51" s="112"/>
+      <c r="C51" s="97"/>
       <c r="D51" s="35" t="s">
         <v>103</v>
       </c>
@@ -2616,22 +2616,22 @@
       <c r="F51" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="G51" s="72" t="s">
+      <c r="G51" s="91" t="s">
         <v>107</v>
       </c>
-      <c r="H51" s="72"/>
-      <c r="I51" s="72"/>
-      <c r="J51" s="88" t="s">
+      <c r="H51" s="91"/>
+      <c r="I51" s="91"/>
+      <c r="J51" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="K51" s="88"/>
-      <c r="L51" s="88"/>
+      <c r="K51" s="93"/>
+      <c r="L51" s="93"/>
     </row>
     <row r="52" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B52" s="41">
         <v>20</v>
       </c>
-      <c r="C52" s="112"/>
+      <c r="C52" s="97"/>
       <c r="D52" s="33" t="s">
         <v>108</v>
       </c>
@@ -2641,35 +2641,35 @@
       <c r="F52" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="G52" s="72" t="s">
+      <c r="G52" s="91" t="s">
         <v>111</v>
       </c>
-      <c r="H52" s="72"/>
-      <c r="I52" s="72"/>
-      <c r="J52" s="82" t="s">
+      <c r="H52" s="91"/>
+      <c r="I52" s="91"/>
+      <c r="J52" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="K52" s="82"/>
-      <c r="L52" s="82"/>
+      <c r="K52" s="92"/>
+      <c r="L52" s="92"/>
     </row>
     <row r="53" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B53" s="109"/>
-      <c r="C53" s="110"/>
-      <c r="D53" s="110"/>
-      <c r="E53" s="110"/>
-      <c r="F53" s="110"/>
-      <c r="G53" s="110"/>
-      <c r="H53" s="110"/>
-      <c r="I53" s="110"/>
-      <c r="J53" s="110"/>
-      <c r="K53" s="110"/>
-      <c r="L53" s="111"/>
+      <c r="B53" s="88"/>
+      <c r="C53" s="89"/>
+      <c r="D53" s="89"/>
+      <c r="E53" s="89"/>
+      <c r="F53" s="89"/>
+      <c r="G53" s="89"/>
+      <c r="H53" s="89"/>
+      <c r="I53" s="89"/>
+      <c r="J53" s="89"/>
+      <c r="K53" s="89"/>
+      <c r="L53" s="90"/>
     </row>
     <row r="54" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B54" s="41">
         <v>21</v>
       </c>
-      <c r="C54" s="86" t="s">
+      <c r="C54" s="95" t="s">
         <v>112</v>
       </c>
       <c r="D54" s="33" t="s">
@@ -2681,22 +2681,22 @@
       <c r="F54" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="G54" s="72" t="s">
+      <c r="G54" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="H54" s="72"/>
-      <c r="I54" s="72"/>
-      <c r="J54" s="88" t="s">
+      <c r="H54" s="91"/>
+      <c r="I54" s="91"/>
+      <c r="J54" s="93" t="s">
         <v>16</v>
       </c>
-      <c r="K54" s="88"/>
-      <c r="L54" s="88"/>
+      <c r="K54" s="93"/>
+      <c r="L54" s="93"/>
     </row>
     <row r="55" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B55" s="41">
         <v>22</v>
       </c>
-      <c r="C55" s="86"/>
+      <c r="C55" s="95"/>
       <c r="D55" s="33" t="s">
         <v>117</v>
       </c>
@@ -2706,22 +2706,22 @@
       <c r="F55" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="G55" s="72" t="s">
+      <c r="G55" s="91" t="s">
         <v>121</v>
       </c>
-      <c r="H55" s="72"/>
-      <c r="I55" s="72"/>
-      <c r="J55" s="81" t="s">
+      <c r="H55" s="91"/>
+      <c r="I55" s="91"/>
+      <c r="J55" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="K55" s="81"/>
-      <c r="L55" s="81"/>
+      <c r="K55" s="94"/>
+      <c r="L55" s="94"/>
     </row>
     <row r="56" spans="2:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B56" s="41">
         <v>23</v>
       </c>
-      <c r="C56" s="86"/>
+      <c r="C56" s="95"/>
       <c r="D56" s="33" t="s">
         <v>118</v>
       </c>
@@ -2731,35 +2731,35 @@
       <c r="F56" s="36" t="s">
         <v>124</v>
       </c>
-      <c r="G56" s="72" t="s">
+      <c r="G56" s="91" t="s">
         <v>123</v>
       </c>
-      <c r="H56" s="72"/>
-      <c r="I56" s="72"/>
-      <c r="J56" s="87" t="s">
+      <c r="H56" s="91"/>
+      <c r="I56" s="91"/>
+      <c r="J56" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="K56" s="87"/>
-      <c r="L56" s="87"/>
+      <c r="K56" s="96"/>
+      <c r="L56" s="96"/>
     </row>
     <row r="57" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="109"/>
-      <c r="C57" s="110"/>
-      <c r="D57" s="110"/>
-      <c r="E57" s="110"/>
-      <c r="F57" s="110"/>
-      <c r="G57" s="110"/>
-      <c r="H57" s="110"/>
-      <c r="I57" s="110"/>
-      <c r="J57" s="110"/>
-      <c r="K57" s="110"/>
-      <c r="L57" s="111"/>
+      <c r="B57" s="88"/>
+      <c r="C57" s="89"/>
+      <c r="D57" s="89"/>
+      <c r="E57" s="89"/>
+      <c r="F57" s="89"/>
+      <c r="G57" s="89"/>
+      <c r="H57" s="89"/>
+      <c r="I57" s="89"/>
+      <c r="J57" s="89"/>
+      <c r="K57" s="89"/>
+      <c r="L57" s="90"/>
     </row>
     <row r="58" spans="2:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B58" s="40">
         <v>24</v>
       </c>
-      <c r="C58" s="95" t="s">
+      <c r="C58" s="80" t="s">
         <v>125</v>
       </c>
       <c r="D58" s="33" t="s">
@@ -2771,22 +2771,22 @@
       <c r="F58" s="36" t="s">
         <v>128</v>
       </c>
-      <c r="G58" s="72" t="s">
+      <c r="G58" s="91" t="s">
         <v>129</v>
       </c>
-      <c r="H58" s="72"/>
-      <c r="I58" s="72"/>
-      <c r="J58" s="82" t="s">
+      <c r="H58" s="91"/>
+      <c r="I58" s="91"/>
+      <c r="J58" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="K58" s="82"/>
-      <c r="L58" s="82"/>
+      <c r="K58" s="92"/>
+      <c r="L58" s="92"/>
     </row>
     <row r="59" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B59" s="40">
         <v>25</v>
       </c>
-      <c r="C59" s="96"/>
+      <c r="C59" s="81"/>
       <c r="D59" s="33" t="s">
         <v>130</v>
       </c>
@@ -2796,22 +2796,22 @@
       <c r="F59" s="36" t="s">
         <v>134</v>
       </c>
-      <c r="G59" s="72" t="s">
+      <c r="G59" s="91" t="s">
         <v>133</v>
       </c>
-      <c r="H59" s="72"/>
-      <c r="I59" s="72"/>
-      <c r="J59" s="88" t="s">
+      <c r="H59" s="91"/>
+      <c r="I59" s="91"/>
+      <c r="J59" s="93" t="s">
         <v>132</v>
       </c>
-      <c r="K59" s="88"/>
-      <c r="L59" s="88"/>
+      <c r="K59" s="93"/>
+      <c r="L59" s="93"/>
     </row>
     <row r="60" spans="2:12" ht="107.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B60" s="40">
         <v>26</v>
       </c>
-      <c r="C60" s="97"/>
+      <c r="C60" s="82"/>
       <c r="D60" s="33" t="s">
         <v>135</v>
       </c>
@@ -2821,29 +2821,29 @@
       <c r="F60" s="34" t="s">
         <v>138</v>
       </c>
-      <c r="G60" s="72" t="s">
+      <c r="G60" s="91" t="s">
         <v>137</v>
       </c>
-      <c r="H60" s="72"/>
-      <c r="I60" s="72"/>
-      <c r="J60" s="82" t="s">
+      <c r="H60" s="91"/>
+      <c r="I60" s="91"/>
+      <c r="J60" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="K60" s="82"/>
-      <c r="L60" s="82"/>
+      <c r="K60" s="92"/>
+      <c r="L60" s="92"/>
     </row>
     <row r="61" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B61" s="61"/>
-      <c r="C61" s="62"/>
-      <c r="D61" s="62"/>
-      <c r="E61" s="62"/>
-      <c r="F61" s="62"/>
-      <c r="G61" s="62"/>
-      <c r="H61" s="62"/>
-      <c r="I61" s="62"/>
-      <c r="J61" s="62"/>
-      <c r="K61" s="62"/>
-      <c r="L61" s="63"/>
+      <c r="B61" s="73"/>
+      <c r="C61" s="74"/>
+      <c r="D61" s="74"/>
+      <c r="E61" s="74"/>
+      <c r="F61" s="74"/>
+      <c r="G61" s="74"/>
+      <c r="H61" s="74"/>
+      <c r="I61" s="74"/>
+      <c r="J61" s="74"/>
+      <c r="K61" s="74"/>
+      <c r="L61" s="75"/>
     </row>
     <row r="62" spans="2:12" ht="81" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B62" s="46">
@@ -2861,35 +2861,35 @@
       <c r="F62" s="33" t="s">
         <v>142</v>
       </c>
-      <c r="G62" s="116" t="s">
+      <c r="G62" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="H62" s="117"/>
-      <c r="I62" s="118"/>
-      <c r="J62" s="103" t="s">
+      <c r="H62" s="77"/>
+      <c r="I62" s="78"/>
+      <c r="J62" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="K62" s="104"/>
-      <c r="L62" s="105"/>
+      <c r="K62" s="68"/>
+      <c r="L62" s="69"/>
     </row>
     <row r="63" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B63" s="122"/>
-      <c r="C63" s="123"/>
-      <c r="D63" s="123"/>
-      <c r="E63" s="123"/>
-      <c r="F63" s="123"/>
-      <c r="G63" s="123"/>
-      <c r="H63" s="123"/>
-      <c r="I63" s="123"/>
-      <c r="J63" s="123"/>
-      <c r="K63" s="123"/>
-      <c r="L63" s="124"/>
+      <c r="B63" s="61"/>
+      <c r="C63" s="62"/>
+      <c r="D63" s="62"/>
+      <c r="E63" s="62"/>
+      <c r="F63" s="62"/>
+      <c r="G63" s="62"/>
+      <c r="H63" s="62"/>
+      <c r="I63" s="62"/>
+      <c r="J63" s="62"/>
+      <c r="K63" s="62"/>
+      <c r="L63" s="63"/>
     </row>
     <row r="64" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B64" s="48">
         <v>28</v>
       </c>
-      <c r="C64" s="120" t="s">
+      <c r="C64" s="59" t="s">
         <v>144</v>
       </c>
       <c r="D64" s="32" t="s">
@@ -2901,22 +2901,22 @@
       <c r="F64" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="G64" s="116" t="s">
+      <c r="G64" s="76" t="s">
         <v>148</v>
       </c>
-      <c r="H64" s="117"/>
-      <c r="I64" s="118"/>
-      <c r="J64" s="106" t="s">
+      <c r="H64" s="77"/>
+      <c r="I64" s="78"/>
+      <c r="J64" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="K64" s="107"/>
-      <c r="L64" s="108"/>
+      <c r="K64" s="65"/>
+      <c r="L64" s="66"/>
     </row>
     <row r="65" spans="2:12" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B65" s="41">
         <v>29</v>
       </c>
-      <c r="C65" s="91"/>
+      <c r="C65" s="60"/>
       <c r="D65" s="35" t="s">
         <v>149</v>
       </c>
@@ -2926,35 +2926,35 @@
       <c r="F65" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="G65" s="116" t="s">
+      <c r="G65" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="H65" s="117"/>
-      <c r="I65" s="118"/>
-      <c r="J65" s="113" t="s">
+      <c r="H65" s="77"/>
+      <c r="I65" s="78"/>
+      <c r="J65" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="K65" s="114"/>
-      <c r="L65" s="115"/>
+      <c r="K65" s="71"/>
+      <c r="L65" s="72"/>
     </row>
     <row r="66" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="61"/>
-      <c r="C66" s="62"/>
-      <c r="D66" s="62"/>
-      <c r="E66" s="62"/>
-      <c r="F66" s="62"/>
-      <c r="G66" s="62"/>
-      <c r="H66" s="62"/>
-      <c r="I66" s="62"/>
-      <c r="J66" s="62"/>
-      <c r="K66" s="62"/>
-      <c r="L66" s="63"/>
+      <c r="B66" s="73"/>
+      <c r="C66" s="74"/>
+      <c r="D66" s="74"/>
+      <c r="E66" s="74"/>
+      <c r="F66" s="74"/>
+      <c r="G66" s="74"/>
+      <c r="H66" s="74"/>
+      <c r="I66" s="74"/>
+      <c r="J66" s="74"/>
+      <c r="K66" s="74"/>
+      <c r="L66" s="75"/>
     </row>
     <row r="67" spans="2:12" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B67" s="40">
         <v>30</v>
       </c>
-      <c r="C67" s="120" t="s">
+      <c r="C67" s="59" t="s">
         <v>153</v>
       </c>
       <c r="D67" s="35" t="s">
@@ -2966,22 +2966,22 @@
       <c r="F67" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="G67" s="116" t="s">
+      <c r="G67" s="76" t="s">
         <v>156</v>
       </c>
-      <c r="H67" s="117"/>
-      <c r="I67" s="118"/>
-      <c r="J67" s="106" t="s">
+      <c r="H67" s="77"/>
+      <c r="I67" s="78"/>
+      <c r="J67" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="K67" s="107"/>
-      <c r="L67" s="108"/>
+      <c r="K67" s="65"/>
+      <c r="L67" s="66"/>
     </row>
     <row r="68" spans="2:12" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B68" s="40">
         <v>31</v>
       </c>
-      <c r="C68" s="91"/>
+      <c r="C68" s="60"/>
       <c r="D68" s="35" t="s">
         <v>158</v>
       </c>
@@ -2991,106 +2991,125 @@
       <c r="F68" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="G68" s="119" t="s">
+      <c r="G68" s="79" t="s">
         <v>160</v>
       </c>
-      <c r="H68" s="119"/>
-      <c r="I68" s="119"/>
-      <c r="J68" s="103" t="s">
+      <c r="H68" s="79"/>
+      <c r="I68" s="79"/>
+      <c r="J68" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="K68" s="104"/>
-      <c r="L68" s="105"/>
+      <c r="K68" s="68"/>
+      <c r="L68" s="69"/>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G69" s="121"/>
-      <c r="H69" s="121"/>
-      <c r="I69" s="121"/>
-      <c r="J69" s="121"/>
-      <c r="K69" s="121"/>
-      <c r="L69" s="121"/>
+      <c r="G69" s="58"/>
+      <c r="H69" s="58"/>
+      <c r="I69" s="58"/>
+      <c r="J69" s="58"/>
+      <c r="K69" s="58"/>
+      <c r="L69" s="58"/>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G70" s="121"/>
-      <c r="H70" s="121"/>
-      <c r="I70" s="121"/>
-      <c r="J70" s="121"/>
-      <c r="K70" s="121"/>
-      <c r="L70" s="121"/>
+      <c r="G70" s="58"/>
+      <c r="H70" s="58"/>
+      <c r="I70" s="58"/>
+      <c r="J70" s="58"/>
+      <c r="K70" s="58"/>
+      <c r="L70" s="58"/>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G71" s="121"/>
-      <c r="H71" s="121"/>
-      <c r="I71" s="121"/>
-      <c r="J71" s="121"/>
-      <c r="K71" s="121"/>
-      <c r="L71" s="121"/>
+      <c r="G71" s="58"/>
+      <c r="H71" s="58"/>
+      <c r="I71" s="58"/>
+      <c r="J71" s="58"/>
+      <c r="K71" s="58"/>
+      <c r="L71" s="58"/>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G72" s="121"/>
-      <c r="H72" s="121"/>
-      <c r="I72" s="121"/>
-      <c r="J72" s="121"/>
-      <c r="K72" s="121"/>
-      <c r="L72" s="121"/>
+      <c r="G72" s="58"/>
+      <c r="H72" s="58"/>
+      <c r="I72" s="58"/>
+      <c r="J72" s="58"/>
+      <c r="K72" s="58"/>
+      <c r="L72" s="58"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G73" s="121"/>
-      <c r="H73" s="121"/>
-      <c r="I73" s="121"/>
-      <c r="J73" s="121"/>
-      <c r="K73" s="121"/>
-      <c r="L73" s="121"/>
+      <c r="G73" s="58"/>
+      <c r="H73" s="58"/>
+      <c r="I73" s="58"/>
+      <c r="J73" s="58"/>
+      <c r="K73" s="58"/>
+      <c r="L73" s="58"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="G74" s="121"/>
-      <c r="H74" s="121"/>
-      <c r="I74" s="121"/>
-      <c r="J74" s="121"/>
-      <c r="K74" s="121"/>
-      <c r="L74" s="121"/>
+      <c r="G74" s="58"/>
+      <c r="H74" s="58"/>
+      <c r="I74" s="58"/>
+      <c r="J74" s="58"/>
+      <c r="K74" s="58"/>
+      <c r="L74" s="58"/>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J75" s="121"/>
-      <c r="K75" s="121"/>
-      <c r="L75" s="121"/>
+      <c r="J75" s="58"/>
+      <c r="K75" s="58"/>
+      <c r="L75" s="58"/>
     </row>
     <row r="76" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="J76" s="121"/>
-      <c r="K76" s="121"/>
-      <c r="L76" s="121"/>
+      <c r="J76" s="58"/>
+      <c r="K76" s="58"/>
+      <c r="L76" s="58"/>
     </row>
   </sheetData>
   <mergeCells count="101">
-    <mergeCell ref="J76:L76"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="B63:L63"/>
-    <mergeCell ref="J71:L71"/>
-    <mergeCell ref="J72:L72"/>
-    <mergeCell ref="J73:L73"/>
-    <mergeCell ref="J74:L74"/>
-    <mergeCell ref="J75:L75"/>
-    <mergeCell ref="J67:L67"/>
-    <mergeCell ref="J68:L68"/>
-    <mergeCell ref="J69:L69"/>
-    <mergeCell ref="J70:L70"/>
-    <mergeCell ref="G69:I69"/>
-    <mergeCell ref="G70:I70"/>
-    <mergeCell ref="G71:I71"/>
-    <mergeCell ref="G72:I72"/>
-    <mergeCell ref="G73:I73"/>
-    <mergeCell ref="G74:I74"/>
-    <mergeCell ref="J62:L62"/>
-    <mergeCell ref="J64:L64"/>
-    <mergeCell ref="J65:L65"/>
-    <mergeCell ref="B61:L61"/>
-    <mergeCell ref="G62:I62"/>
-    <mergeCell ref="G64:I64"/>
-    <mergeCell ref="G65:I65"/>
-    <mergeCell ref="G67:I67"/>
-    <mergeCell ref="G68:I68"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="B66:L66"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="B26:L26"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="E3:F10"/>
+    <mergeCell ref="G27:I27"/>
+    <mergeCell ref="J25:L25"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="G38:I38"/>
+    <mergeCell ref="J38:L38"/>
+    <mergeCell ref="G25:I25"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:L32"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="G29:I29"/>
+    <mergeCell ref="J29:L29"/>
+    <mergeCell ref="G30:I30"/>
+    <mergeCell ref="J30:L30"/>
+    <mergeCell ref="G37:I37"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="J36:L36"/>
+    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="C44:C46"/>
+    <mergeCell ref="G48:I48"/>
+    <mergeCell ref="J48:L48"/>
+    <mergeCell ref="G44:I44"/>
+    <mergeCell ref="J44:L44"/>
+    <mergeCell ref="G45:I45"/>
+    <mergeCell ref="J45:L45"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="J34:L34"/>
+    <mergeCell ref="G39:I39"/>
+    <mergeCell ref="J39:L39"/>
+    <mergeCell ref="G41:I41"/>
+    <mergeCell ref="J41:L41"/>
+    <mergeCell ref="G42:I42"/>
+    <mergeCell ref="J42:L42"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="B35:L35"/>
+    <mergeCell ref="J54:L54"/>
+    <mergeCell ref="G49:I49"/>
+    <mergeCell ref="J49:L49"/>
+    <mergeCell ref="G50:I50"/>
+    <mergeCell ref="G51:I51"/>
+    <mergeCell ref="J51:L51"/>
+    <mergeCell ref="J50:L50"/>
+    <mergeCell ref="G46:I46"/>
+    <mergeCell ref="J46:L46"/>
     <mergeCell ref="C58:C60"/>
     <mergeCell ref="C41:C42"/>
     <mergeCell ref="B40:L40"/>
@@ -3115,54 +3134,35 @@
     <mergeCell ref="G52:I52"/>
     <mergeCell ref="C48:C52"/>
     <mergeCell ref="G54:I54"/>
-    <mergeCell ref="J54:L54"/>
-    <mergeCell ref="G49:I49"/>
-    <mergeCell ref="J49:L49"/>
-    <mergeCell ref="G50:I50"/>
-    <mergeCell ref="G51:I51"/>
-    <mergeCell ref="J51:L51"/>
-    <mergeCell ref="J50:L50"/>
-    <mergeCell ref="G46:I46"/>
-    <mergeCell ref="J46:L46"/>
-    <mergeCell ref="C44:C46"/>
-    <mergeCell ref="G48:I48"/>
-    <mergeCell ref="J48:L48"/>
-    <mergeCell ref="G44:I44"/>
-    <mergeCell ref="J44:L44"/>
-    <mergeCell ref="G45:I45"/>
-    <mergeCell ref="J45:L45"/>
-    <mergeCell ref="G34:I34"/>
-    <mergeCell ref="J34:L34"/>
-    <mergeCell ref="G39:I39"/>
-    <mergeCell ref="J39:L39"/>
-    <mergeCell ref="G41:I41"/>
-    <mergeCell ref="J41:L41"/>
-    <mergeCell ref="G42:I42"/>
-    <mergeCell ref="J42:L42"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="B35:L35"/>
-    <mergeCell ref="C27:C30"/>
-    <mergeCell ref="B26:L26"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="E3:F10"/>
-    <mergeCell ref="G27:I27"/>
-    <mergeCell ref="J25:L25"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="G38:I38"/>
-    <mergeCell ref="J38:L38"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:L32"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="G29:I29"/>
-    <mergeCell ref="J29:L29"/>
-    <mergeCell ref="G30:I30"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="G37:I37"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="J36:L36"/>
-    <mergeCell ref="B33:L33"/>
+    <mergeCell ref="J62:L62"/>
+    <mergeCell ref="J64:L64"/>
+    <mergeCell ref="J65:L65"/>
+    <mergeCell ref="B61:L61"/>
+    <mergeCell ref="G62:I62"/>
+    <mergeCell ref="G64:I64"/>
+    <mergeCell ref="G65:I65"/>
+    <mergeCell ref="G67:I67"/>
+    <mergeCell ref="G68:I68"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="B66:L66"/>
+    <mergeCell ref="J76:L76"/>
+    <mergeCell ref="C64:C65"/>
+    <mergeCell ref="B63:L63"/>
+    <mergeCell ref="J71:L71"/>
+    <mergeCell ref="J72:L72"/>
+    <mergeCell ref="J73:L73"/>
+    <mergeCell ref="J74:L74"/>
+    <mergeCell ref="J75:L75"/>
+    <mergeCell ref="J67:L67"/>
+    <mergeCell ref="J68:L68"/>
+    <mergeCell ref="J69:L69"/>
+    <mergeCell ref="J70:L70"/>
+    <mergeCell ref="G69:I69"/>
+    <mergeCell ref="G70:I70"/>
+    <mergeCell ref="G71:I71"/>
+    <mergeCell ref="G72:I72"/>
+    <mergeCell ref="G73:I73"/>
+    <mergeCell ref="G74:I74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>